<commit_message>
Update weekly ranking [2025-10-22]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -501,7 +501,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>黄昏町プリズナーズ</t>
+          <t>アイドラトリィ</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>アイドラトリィ</t>
+          <t>黄昏町プリズナーズ</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+          <t>JK Biker</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>JK Biker</t>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+          <t>イエティ、とある日々</t>
         </is>
       </c>
     </row>
@@ -841,7 +841,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>イエティ、とある日々</t>
+          <t>東京デスレース</t>
         </is>
       </c>
     </row>
@@ -851,7 +851,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>東京デスレース</t>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update weekly ranking [2025-10-29]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="magapoke_2025-10-22" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="magapoke_2025-10-29" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -858,4 +859,445 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>鉱石令嬢〜没落した悪役令嬢が炭鉱で一山当てるまでのお話〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>英雄と魔女の転生ラブコメ</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-11-05]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="magapoke_2025-10-22" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="magapoke_2025-10-29" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="magapoke_2025-11-05" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1300,4 +1301,455 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>英雄と魔女の転生ラブコメ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>鉱石令嬢〜没落した悪役令嬢が炭鉱で一山当てるまでのお話〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-11-12]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -10,6 +10,7 @@
     <sheet name="magapoke_2025-10-22" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="magapoke_2025-10-29" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="magapoke_2025-11-05" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="magapoke_2025-11-12" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1752,4 +1753,475 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>鉱石令嬢〜没落した悪役令嬢が炭鉱で一山当てるまでのお話〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>英雄と魔女の転生ラブコメ</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-11-19]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -11,6 +11,7 @@
     <sheet name="magapoke_2025-10-29" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="magapoke_2025-11-05" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="magapoke_2025-11-12" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="magapoke_2025-11-19" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2224,4 +2225,465 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>鉱石令嬢〜没落した悪役令嬢が炭鉱で一山当てるまでのお話〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-11-26]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -12,6 +12,7 @@
     <sheet name="magapoke_2025-11-05" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="magapoke_2025-11-12" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="magapoke_2025-11-19" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="magapoke_2025-11-26" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2686,4 +2687,475 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>鉱石令嬢〜没落した悪役令嬢が炭鉱で一山当てるまでのお話〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-12-03]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -13,6 +13,7 @@
     <sheet name="magapoke_2025-11-12" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="magapoke_2025-11-19" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="magapoke_2025-11-26" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="magapoke_2025-12-03" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3158,4 +3159,485 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>鉱石令嬢〜没落した悪役令嬢が炭鉱で一山当てるまでのお話〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-12-10]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -14,6 +14,7 @@
     <sheet name="magapoke_2025-11-19" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="magapoke_2025-11-26" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="magapoke_2025-12-03" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="magapoke_2025-12-10" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3640,4 +3641,485 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>それがメイドのカンナです</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-12-17]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -15,6 +15,7 @@
     <sheet name="magapoke_2025-11-26" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="magapoke_2025-12-03" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="magapoke_2025-12-10" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="magapoke_2025-12-17" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4122,4 +4123,475 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>東京デスレース</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update weekly ranking [2025-12-24]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -16,6 +16,7 @@
     <sheet name="magapoke_2025-12-03" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="magapoke_2025-12-10" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="magapoke_2025-12-17" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="magapoke_2025-12-24" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -868,6 +869,487 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ハナバス　苔石花江のバスケ論</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2025-12-31]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -17,6 +17,7 @@
     <sheet name="magapoke_2025-12-10" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="magapoke_2025-12-17" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="magapoke_2025-12-24" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="magapoke_2025-12-31" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1350,6 +1351,477 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-01-07]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -18,6 +18,7 @@
     <sheet name="magapoke_2025-12-17" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="magapoke_2025-12-24" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="magapoke_2025-12-31" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="magapoke_2026-01-07" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1822,6 +1823,477 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-01-14]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -19,6 +19,7 @@
     <sheet name="magapoke_2025-12-24" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="magapoke_2025-12-31" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="magapoke_2026-01-07" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="magapoke_2026-01-14" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2294,6 +2295,507 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>スルガメテオ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>生きたがりの人狼</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-01-21]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -20,6 +20,7 @@
     <sheet name="magapoke_2025-12-31" sheetId="11" state="visible" r:id="rId11"/>
     <sheet name="magapoke_2026-01-07" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="magapoke_2026-01-14" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="magapoke_2026-01-21" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2796,6 +2797,487 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-01-28]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -21,6 +21,7 @@
     <sheet name="magapoke_2026-01-07" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="magapoke_2026-01-14" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="magapoke_2026-01-21" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="magapoke_2026-01-28" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3278,6 +3279,507 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>邪目さんは邪神です</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>白鳥運子は31画</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>卒業アルバムの彼女たち</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-02-04]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -22,6 +22,7 @@
     <sheet name="magapoke_2026-01-14" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="magapoke_2026-01-21" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="magapoke_2026-01-28" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="magapoke_2026-02-04" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3780,6 +3781,507 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ハンドレッドノート－アグリーダック－</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>邪目さんは邪神です</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>白鳥運子は31画</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-02-11]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -23,6 +23,7 @@
     <sheet name="magapoke_2026-01-21" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="magapoke_2026-01-28" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="magapoke_2026-02-04" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="magapoke_2026-02-11" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4282,6 +4283,547 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ハンドレッドノート－アグリーダック－</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ペンの夢に紅をさす</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>お前がヤったんだろ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>邪目さんは邪神です</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>白鳥運子は31画</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>わが投資術　市場は誰に微笑むか</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ch登録お願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>〈小市民〉 春期限定いちごタルト事件</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-02-18]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -24,6 +24,7 @@
     <sheet name="magapoke_2026-01-28" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="magapoke_2026-02-04" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="magapoke_2026-02-11" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="magapoke_2026-02-18" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4824,6 +4825,547 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>怨霊日和</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ハンドレッドノート－アグリーダック－</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ペンの夢に紅をさす</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>お前がヤったんだろ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>白鳥運子は31画</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>わが投資術　市場は誰に微笑むか</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>邪目さんは邪神です</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>篝家の８兄弟</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ch登録お願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>ナキナギ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>夜鐘のキト</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Update weekly ranking [2026-02-25]
</commit_message>
<xml_diff>
--- a/weekly_ranking.xlsx
+++ b/weekly_ranking.xlsx
@@ -25,6 +25,7 @@
     <sheet name="magapoke_2026-02-04" sheetId="16" state="visible" r:id="rId16"/>
     <sheet name="magapoke_2026-02-11" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="magapoke_2026-02-18" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="magapoke_2026-02-25" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5366,6 +5367,517 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>rank</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>アイドラトリィ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ペンの夢に紅をさす</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>黒月のイェルクナハト</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>あの島の海音荘</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ドリーム☆ジャンボ☆ガール</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>黄昏町プリズナーズ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>K-9~警視庁公安部公安第9課異能対策係~</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>【爆アド】生まれた直後から最強悪霊と脳内バトルしてたら魔力量が測定可能域を超えてました〜悪憑の子の謙虚な覇道〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ゼロとヒャク</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ハードワーカー中田</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>せいぶつ部の田辺くん</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ハンドレッドノート－アグリーダック－</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ともだちづくり</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>怨霊日和</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>普通の本はありません！</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>お母さん冒険者、ログインボーナスでスキル【主婦】に目覚めました。週一貰えるチラシで冒険者生活頑張ります！</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>白鳥運子は31画</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>お前がヤったんだろ！</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>皇女転生　～伝説の大魔導士（♂）、姫騎士となりて伝説の令嬢騎士団を作り無双する～</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>屋根の下のアルテミス</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MYS</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>限界集落を脱村した錬金術士、都会で"最強"なのがバレまくる。～老害どもにはいい加減愛想が尽きました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>わが投資術　市場は誰に微笑むか</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>異世界グルメで成り上がり無双～山に追放されたので、のんびりキャンプを楽しんでいたらいつの間にか強くなっていて、王侯貴族や実力者たちが俺を放っておいてくれません。一方、俺を追放した貴族たちは破滅が始まる～</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>君が監督！</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>その青春</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>鳴るさんだぁ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ナマイキ旭ちゃんをわからせたい</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>明智ナンバーワン</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>春くらり</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>平成転生</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>追放されなかった男　～二度目の人生は土下座から始まりました～</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>じゅーくぼっくす</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>歪みの虜</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>人生逆転ダンジョン</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>JK Biker</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>GURU</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>ルックスＹを選んでしまいました 〜やり込んでいるゲームに転生したはずなのに、未実装のガチャで攻略をすることになった件〜</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>ch登録お願いします！</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>眠れる森のレガ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>ハプスブルク家の華麗なる受難</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>邪目さんは邪神です</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>白銀のキュイジーヌ～明治外交官の料理人～</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>永久のユウグレ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>宇曽田みのりの代用料理</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>花子狩り</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>イエティ、とある日々</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>きゃわるり方程式</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>